<commit_message>
test ganti deskt (#5)
test
</commit_message>
<xml_diff>
--- a/attendance_template.xlsx
+++ b/attendance_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PM\Documents\kerjaan david\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PM\Documents\wong\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -725,9 +725,9 @@
         <f>IFERROR(VLOOKUP(Filling!A2,Master!$A$2:$C$100,2,FALSE),"")</f>
         <v>5</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="6" t="str">
         <f>IF(ISBLANK(Filling!B2)," ",Filling!B2)</f>
-        <v>42380.333333333336</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="6">
         <f>IF(ISBLANK(Filling!C2)," ",Filling!C2)</f>
@@ -1441,7 +1441,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,9 +1473,6 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="7">
-        <v>42380.333333333336</v>
       </c>
       <c r="C2" s="7">
         <v>42380.708333333336</v>

</xml_diff>

<commit_message>
test tambah lagi deskt
tyedzda
</commit_message>
<xml_diff>
--- a/attendance_template.xlsx
+++ b/attendance_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
   <si>
     <t>Employee_Id</t>
   </si>
@@ -1438,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,35 +1499,99 @@
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42380.708333333336</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B5" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C5" s="7">
+        <v>42380.708333333336</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
+      <c r="B6" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C6" s="7">
+        <v>42380.708333333336</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
+      <c r="B7" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C7" s="7">
+        <v>42380.708333333336</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="B8" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C8" s="7">
+        <v>42380.708333333336</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="B9" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C9" s="7">
+        <v>42380.708333333336</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>50</v>
+      </c>
+      <c r="B10" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C10" s="7">
+        <v>42380.708333333336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C11" s="7">
+        <v>42380.708333333336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="7">
+        <v>42380.333333333336</v>
+      </c>
+      <c r="C12" s="7">
+        <v>42380.708333333336</v>
       </c>
     </row>
   </sheetData>
@@ -1554,7 +1618,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8">
       <formula1>allEmployee</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A12">
       <formula1>allEmployee</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>